<commit_message>
twaeked change log and examples
</commit_message>
<xml_diff>
--- a/docs/Examples/Fitting_Fermi_Diads/Example1b_CO2_Fluid_Inclusions/PseudoVoigt.xlsx
+++ b/docs/Examples/Fitting_Fermi_Diads/Example1b_CO2_Fluid_Inclusions/PseudoVoigt.xlsx
@@ -620,63 +620,63 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9976777972548549</v>
+        <v>0.997677963090024</v>
       </c>
       <c r="D2" t="n">
-        <v>3.820296003693668e-05</v>
+        <v>3.789130113614438e-05</v>
       </c>
       <c r="E2" t="n">
-        <v>331.2468567065976</v>
+        <v>331.2468016463672</v>
       </c>
       <c r="F2" t="n">
-        <v>1447.583483554174</v>
+        <v>1447.583428519429</v>
       </c>
       <c r="G2" t="n">
-        <v>1116.336626847577</v>
+        <v>1116.336626873062</v>
       </c>
       <c r="H2" t="n">
-        <v>46682.92570200779</v>
+        <v>46708.45839110907</v>
       </c>
       <c r="I2" t="n">
-        <v>4597.466622049759</v>
+        <v>4597.466859655824</v>
       </c>
       <c r="J2" t="n">
-        <v>119.1017680030098</v>
+        <v>119.5719141440429</v>
       </c>
       <c r="K2" t="n">
-        <v>11.72070230557635</v>
+        <v>11.72069730627138</v>
       </c>
       <c r="L2" t="n">
-        <v>3.820296003693668e-05</v>
+        <v>3.789130113614438e-05</v>
       </c>
       <c r="M2" t="n">
-        <v>0.4114408752684049</v>
+        <v>0.4113311823267408</v>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
-        <v>0.00254</v>
+        <v>0.001961902034617951</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4048831178384279</v>
+        <v>0.4068401668521797</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.4154144231256527</v>
+        <v>0.4154143515655463</v>
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
-        <v>0.0123970788943553</v>
+        <v>0.01239709188923505</v>
       </c>
       <c r="T2" t="n">
-        <v>0.3629131935521701</v>
+        <v>0.3629135192468673</v>
       </c>
       <c r="U2" t="n">
-        <v>0.997632810503445</v>
+        <v>0.9976347172963363</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9977227880636678</v>
+        <v>0.9977212126331396</v>
       </c>
       <c r="W2" t="n">
-        <v>130.8224703085862</v>
+        <v>131.2926114503143</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
@@ -740,63 +740,63 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9976720597815372</v>
+        <v>0.9976721691882303</v>
       </c>
       <c r="D3" t="n">
-        <v>3.55141706454311e-05</v>
+        <v>3.507449044370555e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>331.24876166122</v>
+        <v>331.248725335829</v>
       </c>
       <c r="F3" t="n">
-        <v>1447.602850669165</v>
+        <v>1447.60280615436</v>
       </c>
       <c r="G3" t="n">
-        <v>1116.354089007945</v>
+        <v>1116.354080818531</v>
       </c>
       <c r="H3" t="n">
-        <v>46630.82592613831</v>
+        <v>46656.49410210855</v>
       </c>
       <c r="I3" t="n">
-        <v>4618.53904943576</v>
+        <v>4618.306479344215</v>
       </c>
       <c r="J3" t="n">
-        <v>126.1395892928885</v>
+        <v>126.6308857560833</v>
       </c>
       <c r="K3" t="n">
-        <v>12.56166502823557</v>
+        <v>12.55986337145032</v>
       </c>
       <c r="L3" t="n">
-        <v>3.55141706454311e-05</v>
+        <v>3.507449044370555e-05</v>
       </c>
       <c r="M3" t="n">
-        <v>0.413588416755558</v>
+        <v>0.4134911095642975</v>
       </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="n">
-        <v>0.00275</v>
+        <v>0.002044577747540558</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4134535315146298</v>
+        <v>0.4154159704865861</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.4228020513747158</v>
+        <v>0.4228271923107911</v>
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
-        <v>0.01143808486257576</v>
+        <v>0.01143706524846398</v>
       </c>
       <c r="T3" t="n">
-        <v>0.346110521780603</v>
+        <v>0.3459185720153358</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9976293292079543</v>
+        <v>0.9976315661259776</v>
       </c>
       <c r="V3" t="n">
-        <v>0.9977147940157585</v>
+        <v>0.9977127755556626</v>
       </c>
       <c r="W3" t="n">
-        <v>138.701254321124</v>
+        <v>139.1907491275336</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
@@ -860,63 +860,63 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9976602992577229</v>
+        <v>0.9976603828406621</v>
       </c>
       <c r="D4" t="n">
-        <v>3.672670265965171e-05</v>
+        <v>3.625817038997172e-05</v>
       </c>
       <c r="E4" t="n">
-        <v>331.2526664562217</v>
+        <v>331.2526387042212</v>
       </c>
       <c r="F4" t="n">
-        <v>1447.62470846539</v>
+        <v>1447.624676270078</v>
       </c>
       <c r="G4" t="n">
-        <v>1116.372042009168</v>
+        <v>1116.372037565857</v>
       </c>
       <c r="H4" t="n">
-        <v>44940.54075914595</v>
+        <v>44966.09125519858</v>
       </c>
       <c r="I4" t="n">
-        <v>4501.199855470801</v>
+        <v>4501.07228842146</v>
       </c>
       <c r="J4" t="n">
-        <v>124.5049356960575</v>
+        <v>125.0162487015378</v>
       </c>
       <c r="K4" t="n">
-        <v>13.1130663661634</v>
+        <v>13.11176800510184</v>
       </c>
       <c r="L4" t="n">
-        <v>3.672670265965172e-05</v>
+        <v>3.625817038997172e-05</v>
       </c>
       <c r="M4" t="n">
-        <v>0.4138258581280082</v>
+        <v>0.4137356048528412</v>
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>0.00289</v>
+        <v>0.002148399943571912</v>
       </c>
       <c r="P4" t="n">
-        <v>0.4202757557542137</v>
+        <v>0.4223033224530864</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.4173876077687431</v>
+        <v>0.4174042203422526</v>
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="n">
-        <v>0.01181757302234964</v>
+        <v>0.01181690488845993</v>
       </c>
       <c r="T4" t="n">
-        <v>0.3467561388231087</v>
+        <v>0.3466455613965865</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9976160052437232</v>
+        <v>0.997618324174933</v>
       </c>
       <c r="V4" t="n">
-        <v>0.9977045972051936</v>
+        <v>0.9977024450528494</v>
       </c>
       <c r="W4" t="n">
-        <v>137.6180020622209</v>
+        <v>138.1280167066397</v>
       </c>
       <c r="X4" t="inlineStr">
         <is>
@@ -980,63 +980,63 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9976370900488032</v>
+        <v>0.9976371141494025</v>
       </c>
       <c r="D5" t="n">
-        <v>3.133687321987576e-05</v>
+        <v>3.081009375132641e-05</v>
       </c>
       <c r="E5" t="n">
-        <v>331.2603727779069</v>
+        <v>331.2603647754245</v>
       </c>
       <c r="F5" t="n">
-        <v>1447.661848535337</v>
+        <v>1447.661843630309</v>
       </c>
       <c r="G5" t="n">
-        <v>1116.40147575743</v>
+        <v>1116.401478854885</v>
       </c>
       <c r="H5" t="n">
-        <v>45431.56888359049</v>
+        <v>45456.77684533728</v>
       </c>
       <c r="I5" t="n">
-        <v>4766.487748706169</v>
+        <v>4766.617979168981</v>
       </c>
       <c r="J5" t="n">
-        <v>119.7467600743447</v>
+        <v>120.2870410475835</v>
       </c>
       <c r="K5" t="n">
-        <v>13.5299649394032</v>
+        <v>13.53173955983582</v>
       </c>
       <c r="L5" t="n">
-        <v>3.133687321987576e-05</v>
+        <v>3.081009375132641e-05</v>
       </c>
       <c r="M5" t="n">
-        <v>0.4189172301400295</v>
+        <v>0.4188400336602033</v>
       </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>0.00281</v>
+        <v>0.00207296107132909</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4041124382672924</v>
+        <v>0.4060749588531597</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.4178737452767803</v>
+        <v>0.4178537556066292</v>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="n">
-        <v>0.009993102191158117</v>
+        <v>0.009993427511747251</v>
       </c>
       <c r="T5" t="n">
-        <v>0.3537671877101221</v>
+        <v>0.3538787377604689</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9975985332004269</v>
+        <v>0.9976007758491043</v>
       </c>
       <c r="V5" t="n">
-        <v>0.9976756498777132</v>
+        <v>0.9976734550970926</v>
       </c>
       <c r="W5" t="n">
-        <v>133.2767250137479</v>
+        <v>133.8187806074194</v>
       </c>
       <c r="X5" t="inlineStr">
         <is>
@@ -1100,63 +1100,63 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9976267202081073</v>
+        <v>0.9976267020778394</v>
       </c>
       <c r="D6" t="n">
-        <v>2.799703337055771e-05</v>
+        <v>2.735640832469095e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>331.2638160670901</v>
+        <v>331.2638220872796</v>
       </c>
       <c r="F6" t="n">
-        <v>1447.681417025652</v>
+        <v>1447.68142542972</v>
       </c>
       <c r="G6" t="n">
-        <v>1116.417600958562</v>
+        <v>1116.41760334244</v>
       </c>
       <c r="H6" t="n">
-        <v>44827.9691712049</v>
+        <v>44852.64703610058</v>
       </c>
       <c r="I6" t="n">
-        <v>4825.845692145009</v>
+        <v>4826.049369025101</v>
       </c>
       <c r="J6" t="n">
-        <v>118.1176401635898</v>
+        <v>118.6625581292928</v>
       </c>
       <c r="K6" t="n">
-        <v>15.13350650930987</v>
+        <v>15.14051744672575</v>
       </c>
       <c r="L6" t="n">
-        <v>2.799703337055771e-05</v>
+        <v>2.735640832469094e-05</v>
       </c>
       <c r="M6" t="n">
-        <v>0.4186457397689967</v>
+        <v>0.4185683107223698</v>
       </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>0.00287</v>
+        <v>0.002086874027805218</v>
       </c>
       <c r="P6" t="n">
-        <v>0.4035300751118815</v>
+        <v>0.4054751808071732</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.4208030978983725</v>
+        <v>0.4207737288794502</v>
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="n">
-        <v>0.008819165019953149</v>
+        <v>0.008818628863412906</v>
       </c>
       <c r="T6" t="n">
-        <v>0.3417541860174331</v>
+        <v>0.3419238068643196</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9975915186215827</v>
+        <v>0.9975938603909323</v>
       </c>
       <c r="V6" t="n">
-        <v>0.9976619242790062</v>
+        <v>0.9976595459271734</v>
       </c>
       <c r="W6" t="n">
-        <v>133.2511466728996</v>
+        <v>133.8030755760185</v>
       </c>
       <c r="X6" t="inlineStr">
         <is>
@@ -1220,63 +1220,63 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9976187103018689</v>
+        <v>0.9976186448894745</v>
       </c>
       <c r="D7" t="n">
-        <v>2.713601064308329e-05</v>
+        <v>2.640795616512301e-05</v>
       </c>
       <c r="E7" t="n">
-        <v>331.2664757927744</v>
+        <v>331.2664975134323</v>
       </c>
       <c r="F7" t="n">
-        <v>1447.700543698599</v>
+        <v>1447.700564549888</v>
       </c>
       <c r="G7" t="n">
-        <v>1116.434067905825</v>
+        <v>1116.434067036456</v>
       </c>
       <c r="H7" t="n">
-        <v>44686.18175345768</v>
+        <v>44710.71958289205</v>
       </c>
       <c r="I7" t="n">
-        <v>4641.502572567449</v>
+        <v>4641.207546625555</v>
       </c>
       <c r="J7" t="n">
-        <v>118.5309890733974</v>
+        <v>119.085833272801</v>
       </c>
       <c r="K7" t="n">
-        <v>13.95485095239556</v>
+        <v>13.95164970143268</v>
       </c>
       <c r="L7" t="n">
-        <v>2.713601064308329e-05</v>
+        <v>2.640795616512301e-05</v>
       </c>
       <c r="M7" t="n">
-        <v>0.4194499232246681</v>
+        <v>0.4193689835665058</v>
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>0.00296</v>
+        <v>0.002112949713188917</v>
       </c>
       <c r="P7" t="n">
-        <v>0.4050007708985622</v>
+        <v>0.4069321082466584</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.430977415014005</v>
+        <v>0.4310228552161054</v>
       </c>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="n">
-        <v>0.008487934176223004</v>
+        <v>0.008489063097475182</v>
       </c>
       <c r="T7" t="n">
-        <v>0.3055811487320741</v>
+        <v>0.305319665793264</v>
       </c>
       <c r="U7" t="n">
-        <v>0.9975842357036222</v>
+        <v>0.9975867176428636</v>
       </c>
       <c r="V7" t="n">
-        <v>0.9976531872829499</v>
+        <v>0.9976505741797809</v>
       </c>
       <c r="W7" t="n">
-        <v>132.4858400257929</v>
+        <v>133.0374829742337</v>
       </c>
       <c r="X7" t="inlineStr">
         <is>
@@ -1340,63 +1340,63 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9976038119728091</v>
+        <v>0.9976037012348412</v>
       </c>
       <c r="D8" t="n">
-        <v>2.70518694841627e-05</v>
+        <v>2.619841071991989e-05</v>
       </c>
       <c r="E8" t="n">
-        <v>331.2714229640899</v>
+        <v>331.2714597365318</v>
       </c>
       <c r="F8" t="n">
-        <v>1447.727487920141</v>
+        <v>1447.727525712897</v>
       </c>
       <c r="G8" t="n">
-        <v>1116.456064956051</v>
+        <v>1116.456065976366</v>
       </c>
       <c r="H8" t="n">
-        <v>45554.91418330932</v>
+        <v>45580.57290947381</v>
       </c>
       <c r="I8" t="n">
-        <v>4807.200805908469</v>
+        <v>4807.138936609352</v>
       </c>
       <c r="J8" t="n">
-        <v>120.0039602307503</v>
+        <v>120.6288937242428</v>
       </c>
       <c r="K8" t="n">
-        <v>13.2512282603179</v>
+        <v>13.25113063849876</v>
       </c>
       <c r="L8" t="n">
-        <v>2.705186948416269e-05</v>
+        <v>2.619841071991989e-05</v>
       </c>
       <c r="M8" t="n">
-        <v>0.4203562292693982</v>
+        <v>0.4202625593096239</v>
       </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>0.00312</v>
+        <v>0.002176955563387554</v>
       </c>
       <c r="P8" t="n">
-        <v>0.3977579615116462</v>
+        <v>0.399731134980214</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4370841588477775</v>
+        <v>0.4370924994946145</v>
       </c>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="n">
-        <v>0.008400850239209489</v>
+        <v>0.008401320537696648</v>
       </c>
       <c r="T8" t="n">
-        <v>0.280750784160972</v>
+        <v>0.280698927497818</v>
       </c>
       <c r="U8" t="n">
-        <v>0.9975691188371361</v>
+        <v>0.9975718464217815</v>
       </c>
       <c r="V8" t="n">
-        <v>0.9976385075216594</v>
+        <v>0.997635558082364</v>
       </c>
       <c r="W8" t="n">
-        <v>133.2551884910682</v>
+        <v>133.8800243627416</v>
       </c>
       <c r="X8" t="inlineStr">
         <is>
@@ -1460,63 +1460,63 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9975833720074658</v>
+        <v>0.9975832338571962</v>
       </c>
       <c r="D9" t="n">
-        <v>3.011535043927592e-05</v>
+        <v>2.931386485278933e-05</v>
       </c>
       <c r="E9" t="n">
-        <v>331.278210543549</v>
+        <v>331.2782564205972</v>
       </c>
       <c r="F9" t="n">
-        <v>1447.755280728591</v>
+        <v>1447.755332045013</v>
       </c>
       <c r="G9" t="n">
-        <v>1116.477070185042</v>
+        <v>1116.477075624416</v>
       </c>
       <c r="H9" t="n">
-        <v>46863.93701623962</v>
+        <v>46890.16841601417</v>
       </c>
       <c r="I9" t="n">
-        <v>4402.313000636223</v>
+        <v>4402.013476330178</v>
       </c>
       <c r="J9" t="n">
-        <v>123.4122020795353</v>
+        <v>124.0622908978741</v>
       </c>
       <c r="K9" t="n">
-        <v>14.63220645908284</v>
+        <v>14.63063901418081</v>
       </c>
       <c r="L9" t="n">
-        <v>3.011535043927592e-05</v>
+        <v>2.931386485278933e-05</v>
       </c>
       <c r="M9" t="n">
-        <v>0.4233768957524429</v>
+        <v>0.4232655949531891</v>
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>0.00314</v>
+        <v>0.002149523804893702</v>
       </c>
       <c r="P9" t="n">
-        <v>0.3951333860325856</v>
+        <v>0.3970859917496964</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.4439402344671336</v>
+        <v>0.4439784987947744</v>
       </c>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="n">
-        <v>0.009469537345080405</v>
+        <v>0.009470161696208255</v>
       </c>
       <c r="T9" t="n">
-        <v>0.2382681964002549</v>
+        <v>0.2379996211213599</v>
       </c>
       <c r="U9" t="n">
-        <v>0.9975454021513104</v>
+        <v>0.9975482445494183</v>
       </c>
       <c r="V9" t="n">
-        <v>0.9976213447542465</v>
+        <v>0.9976182256195812</v>
       </c>
       <c r="W9" t="n">
-        <v>138.0444085386182</v>
+        <v>138.692929912055</v>
       </c>
       <c r="X9" t="inlineStr">
         <is>
@@ -1580,63 +1580,63 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.9975758836115708</v>
+        <v>0.9975757172569771</v>
       </c>
       <c r="D10" t="n">
-        <v>3.319493391647526e-05</v>
+        <v>3.242554057759752e-05</v>
       </c>
       <c r="E10" t="n">
-        <v>331.2806973141624</v>
+        <v>331.2807525581552</v>
       </c>
       <c r="F10" t="n">
-        <v>1447.769583255917</v>
+        <v>1447.769638079903</v>
       </c>
       <c r="G10" t="n">
-        <v>1116.488885941754</v>
+        <v>1116.488885521748</v>
       </c>
       <c r="H10" t="n">
-        <v>49165.1742030134</v>
+        <v>49191.44110915018</v>
       </c>
       <c r="I10" t="n">
-        <v>4322.409418499949</v>
+        <v>4322.430490424518</v>
       </c>
       <c r="J10" t="n">
-        <v>128.9423951742382</v>
+        <v>129.5949813472934</v>
       </c>
       <c r="K10" t="n">
-        <v>15.08572350489327</v>
+        <v>15.08669094085558</v>
       </c>
       <c r="L10" t="n">
-        <v>3.319493391647526e-05</v>
+        <v>3.242554057759752e-05</v>
       </c>
       <c r="M10" t="n">
-        <v>0.4230824644631638</v>
+        <v>0.4229639667734412</v>
       </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>0.00316</v>
+        <v>0.002108440016721441</v>
       </c>
       <c r="P10" t="n">
-        <v>0.3913731837809407</v>
+        <v>0.3932426057399453</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.4543415922418678</v>
+        <v>0.4543394629788884</v>
       </c>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="n">
-        <v>0.0105330389154052</v>
+        <v>0.01053300200787734</v>
       </c>
       <c r="T10" t="n">
-        <v>0.228026922051465</v>
+        <v>0.2280451654286512</v>
       </c>
       <c r="U10" t="n">
-        <v>0.9975346518678617</v>
+        <v>0.9975376519172418</v>
       </c>
       <c r="V10" t="n">
-        <v>0.9976171187639373</v>
+        <v>0.9976137855019169</v>
       </c>
       <c r="W10" t="n">
-        <v>144.0281186791315</v>
+        <v>144.681672288149</v>
       </c>
       <c r="X10" t="inlineStr">
         <is>
@@ -1700,63 +1700,63 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.9975700120419233</v>
+        <v>0.9975698417594873</v>
       </c>
       <c r="D11" t="n">
-        <v>3.237068021717647e-05</v>
+        <v>3.16410132567224e-05</v>
       </c>
       <c r="E11" t="n">
-        <v>331.2826471900244</v>
+        <v>331.2827037390637</v>
       </c>
       <c r="F11" t="n">
-        <v>1447.782005064451</v>
+        <v>1447.782064648375</v>
       </c>
       <c r="G11" t="n">
-        <v>1116.499357874427</v>
+        <v>1116.499360909312</v>
       </c>
       <c r="H11" t="n">
-        <v>48792.80313976954</v>
+        <v>48819.08900488963</v>
       </c>
       <c r="I11" t="n">
-        <v>4614.105495822576</v>
+        <v>4613.979699295842</v>
       </c>
       <c r="J11" t="n">
-        <v>122.3242753514026</v>
+        <v>122.976872173722</v>
       </c>
       <c r="K11" t="n">
-        <v>15.16387060697392</v>
+        <v>15.16246746501848</v>
       </c>
       <c r="L11" t="n">
-        <v>3.237068021717647e-05</v>
+        <v>3.16410132567224e-05</v>
       </c>
       <c r="M11" t="n">
-        <v>0.4234179882475531</v>
+        <v>0.4232857045363292</v>
       </c>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>0.00306</v>
+        <v>0.002058472253117562</v>
       </c>
       <c r="P11" t="n">
-        <v>0.3910597179638211</v>
+        <v>0.3929510585828793</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.4516970534099738</v>
+        <v>0.4517106241735679</v>
       </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="n">
-        <v>0.01027799804083842</v>
+        <v>0.01027801247799601</v>
       </c>
       <c r="T11" t="n">
-        <v>0.2525646905223139</v>
+        <v>0.2524598166617361</v>
       </c>
       <c r="U11" t="n">
-        <v>0.9975298498079659</v>
+        <v>0.997532695096764</v>
       </c>
       <c r="V11" t="n">
-        <v>0.9976101775100096</v>
+        <v>0.9976069911888886</v>
       </c>
       <c r="W11" t="n">
-        <v>137.4881459583765</v>
+        <v>138.1393396387405</v>
       </c>
       <c r="X11" t="inlineStr">
         <is>

</xml_diff>